<commit_message>
Everything working.  Minor LCD bug still present.
</commit_message>
<xml_diff>
--- a/sinemif mod.xlsx
+++ b/sinemif mod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Desktop\EE316-Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCE285A-4E34-450E-9D65-2B2209480A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB2F108-75E5-48F1-9F19-A7E4E8062AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1890" windowWidth="29040" windowHeight="15720" xr2:uid="{5C1909C6-2207-40F4-99C6-149E3CC36629}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{5C1909C6-2207-40F4-99C6-149E3CC36629}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5218,15 +5218,15 @@
   <dimension ref="A1:F256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>0</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>0 : 16384;</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>1 : 16786;</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>2 : 17187;</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>3 : 17589;</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>4 : 17989;</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>5 : 18389;</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>6 : 18788;</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>7 : 19185;</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>8 : 19580;</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>9 : 19973;</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>10 : 20364;</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>11 : 20753;</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>12 : 21140;</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>13 : 21523;</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>14 : 21903;</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>15 : 22280;</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>16 : 22653;</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>17 : 23023;</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>18 : 23389;</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>19 : 23750;</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>20 : 24107;</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>21 : 24459;</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>22 : 24807;</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>23 : 25149;</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>24 : 25486;</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>25 : 25818;</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>26 : 26143;</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>27 : 26463;</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>28 : 26777;</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>29 : 27085;</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>30 : 27386;</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>31 : 27681;</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>32 : 27969;</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>33 : 28250;</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>34 : 28523;</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>35 : 28790;</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>36 : 29049;</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>37 : 29300;</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>38 : 29543;</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>39 : 29779;</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>40 : 30006;</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>41 : 30226;</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>42 : 30437;</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>43 : 30639;</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>44 : 30833;</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>45 : 31018;</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>46 : 31194;</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>47 : 31362;</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>48 : 31520;</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>49 : 31670;</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>50 : 31810;</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>51 : 31941;</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>52 : 32062;</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>53 : 32174;</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>54 : 32276;</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>55 : 32369;</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>56 : 32453;</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>57 : 32526;</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>58 : 32590;</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>59 : 32644;</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>60 : 32675;</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>61 : 32675;</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>62 : 32675;</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>63 : 32675;</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>64 : 32675;</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>65 : 32675;</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>66 : 32675;</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>67 : 32675;</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>68 : 32675;</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>69 : 32644;</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>70 : 32590;</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>71 : 32526;</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>72 : 32453;</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>73 : 32369;</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>74 : 32276;</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>75 : 32174;</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>76 : 32062;</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>77 : 31941;</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>78 : 31810;</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>79 : 31670;</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>80 : 31520;</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>81 : 31362;</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7218,7 +7218,7 @@
         <v>82 : 31194;</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>83 : 31018;</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>84 : 30833;</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>85 : 30639;</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>86 : 30437;</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>87 : 30226;</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>88 : 30006;</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>89 : 29779;</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>90 : 29543;</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>91 : 29300;</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>92 : 29049;</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>93 : 28790;</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>94 : 28523;</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>95 : 28250;</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>96 : 27969;</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>97 : 27681;</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>98 : 27386;</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>99 : 27085;</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>100 : 26777;</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>101 : 26463;</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>102 : 26143;</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>103 : 25818;</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>104 : 25486;</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>105 : 25149;</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>106 : 24807;</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>107 : 24459;</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>108 : 24107;</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>109 : 23750;</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>110 : 23389;</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>111 : 23023;</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7938,7 +7938,7 @@
         <v>112 : 22653;</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>113 : 22280;</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>114 : 21903;</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>115 : 21523;</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>116 : 21140;</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>117 : 20753;</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -8082,7 +8082,7 @@
         <v>118 : 20364;</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>119 : 19973;</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>120 : 19580;</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>121 : 19185;</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>122 : 18788;</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>123 : 18389;</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>124 : 17989;</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>125 : 17589;</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>126 : 17187;</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>127 : 16786;</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>128 : 16384;</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>129 : 15981;</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>130</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>130 : 15580;</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>131 : 15178;</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>132 : 14778;</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>133 : 14378;</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>134 : 13979;</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>135 : 13582;</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>136 : 13187;</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>137 : 12794;</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -8562,7 +8562,7 @@
         <v>138 : 12403;</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>139 : 12014;</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>140 : 11627;</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>141 : 11244;</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>142 : 10864;</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>143 : 10487;</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -8706,7 +8706,7 @@
         <v>144 : 10114;</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>145 : 9744;</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>146 : 9378;</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -8778,7 +8778,7 @@
         <v>147 : 9017;</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>148 : 8660;</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>149 : 8308;</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>150 : 7960;</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>151 : 7618;</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>152 : 7281;</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -8922,7 +8922,7 @@
         <v>153 : 6949;</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>154 : 6624;</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>155 : 6304;</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>156 : 5990;</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -9018,7 +9018,7 @@
         <v>157 : 5682;</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>158 : 5381;</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>159 : 5086;</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>160 : 4798;</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>161 : 4517;</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>162 : 4244;</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>163 : 3977;</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>164 : 3718;</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>165 : 3467;</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>166 : 3224;</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -9258,7 +9258,7 @@
         <v>167 : 2988;</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>168 : 2761;</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -9306,7 +9306,7 @@
         <v>169 : 2541;</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>170 : 2330;</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>171 : 2128;</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>172 : 1934;</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -9402,7 +9402,7 @@
         <v>173 : 1749;</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>174 : 1573;</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -9450,7 +9450,7 @@
         <v>175 : 1405;</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -9474,7 +9474,7 @@
         <v>176 : 1247;</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>177 : 1097;</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>178</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>178 : 957;</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -9546,7 +9546,7 @@
         <v>179 : 826;</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>180 : 705;</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>181 : 593;</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>182 : 491;</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>183 : 398;</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>184 : 314;</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>185 : 241;</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -9714,7 +9714,7 @@
         <v>186 : 177;</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>187 : 123;</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>188 : 78;</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>189 : 44;</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -9810,7 +9810,7 @@
         <v>190 : 19;</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -9834,7 +9834,7 @@
         <v>191 : 4;</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -9858,7 +9858,7 @@
         <v>192 : 0;</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>193 : 4;</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -9906,7 +9906,7 @@
         <v>194 : 19;</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -9930,7 +9930,7 @@
         <v>195 : 44;</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>196 : 78;</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -9978,7 +9978,7 @@
         <v>197 : 123;</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -10002,7 +10002,7 @@
         <v>198 : 177;</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>199 : 241;</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>200 : 314;</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -10074,7 +10074,7 @@
         <v>201 : 398;</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>202 : 491;</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>203</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>203 : 593;</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>204</v>
       </c>
@@ -10146,7 +10146,7 @@
         <v>204 : 705;</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -10170,7 +10170,7 @@
         <v>205 : 826;</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -10194,7 +10194,7 @@
         <v>206 : 957;</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>207</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>207 : 1097;</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>208</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>208 : 1247;</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -10266,7 +10266,7 @@
         <v>209 : 1405;</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -10290,7 +10290,7 @@
         <v>210 : 1573;</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>211</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>211 : 1749;</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>212</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>212 : 1934;</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -10362,7 +10362,7 @@
         <v>213 : 2128;</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>214</v>
       </c>
@@ -10386,7 +10386,7 @@
         <v>214 : 2330;</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>215</v>
       </c>
@@ -10410,7 +10410,7 @@
         <v>215 : 2541;</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>216</v>
       </c>
@@ -10434,7 +10434,7 @@
         <v>216 : 2761;</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>217</v>
       </c>
@@ -10458,7 +10458,7 @@
         <v>217 : 2988;</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>218</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>218 : 3224;</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>219</v>
       </c>
@@ -10506,7 +10506,7 @@
         <v>219 : 3467;</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>220</v>
       </c>
@@ -10530,7 +10530,7 @@
         <v>220 : 3718;</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>221</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>221 : 3977;</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>222</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>222 : 4244;</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>223</v>
       </c>
@@ -10602,7 +10602,7 @@
         <v>223 : 4517;</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>224</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>224 : 4798;</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>225</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>225 : 5086;</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>226</v>
       </c>
@@ -10674,7 +10674,7 @@
         <v>226 : 5381;</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>227</v>
       </c>
@@ -10698,7 +10698,7 @@
         <v>227 : 5682;</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>228</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>228 : 5990;</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>229</v>
       </c>
@@ -10746,7 +10746,7 @@
         <v>229 : 6304;</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>230</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>230 : 6624;</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>231</v>
       </c>
@@ -10794,7 +10794,7 @@
         <v>231 : 6949;</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>232</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>232 : 7281;</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>233</v>
       </c>
@@ -10842,7 +10842,7 @@
         <v>233 : 7618;</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>234</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>234 : 7960;</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>235</v>
       </c>
@@ -10890,7 +10890,7 @@
         <v>235 : 8308;</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>236</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>236 : 8660;</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>237</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>237 : 9017;</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>238</v>
       </c>
@@ -10962,7 +10962,7 @@
         <v>238 : 9378;</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>239</v>
       </c>
@@ -10986,7 +10986,7 @@
         <v>239 : 9744;</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>240</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>240 : 10114;</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>241</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>241 : 10487;</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>242</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>242 : 10864;</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>243</v>
       </c>
@@ -11082,7 +11082,7 @@
         <v>243 : 11244;</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>244</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>244 : 11627;</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>245</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>245 : 12014;</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>246</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>246 : 12403;</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>247</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>247 : 12794;</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>248</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>248 : 13187;</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>249</v>
       </c>
@@ -11226,7 +11226,7 @@
         <v>249 : 13582;</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>250</v>
       </c>
@@ -11250,7 +11250,7 @@
         <v>250 : 13979;</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>251</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>251 : 14378;</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>252</v>
       </c>
@@ -11298,7 +11298,7 @@
         <v>252 : 14778;</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>253</v>
       </c>
@@ -11322,7 +11322,7 @@
         <v>253 : 15178;</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>254</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>254 : 15580;</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>255</v>
       </c>

</xml_diff>